<commit_message>
cleaning up, don't send variable that is always 0, fixing spec tests
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/multipage-no-mods/manifest.xlsx
+++ b/spec/fixtures/files/multipage-no-mods/manifest.xlsx
@@ -381,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -457,7 +457,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="5" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>